<commit_message>
updated Formula after Level 60
</commit_message>
<xml_diff>
--- a/documentation/Leveling-Calculator.xlsx
+++ b/documentation/Leveling-Calculator.xlsx
@@ -24,27 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Level</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Formula</t>
   </si>
   <si>
-    <t>Time in Minutes</t>
+    <t>Hours</t>
   </si>
   <si>
-    <t>Hours</t>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>LEVEL</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula Change </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -62,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -82,13 +91,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,41 +416,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <f>600*1.16^A2</f>
         <v>696</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <f>B2/60</f>
         <v>11.6</v>
       </c>
@@ -445,17 +464,21 @@
         <f>C2/60</f>
         <v>0.19333333333333333</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <f>D2/24</f>
+        <v>8.0555555555555554E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f t="shared" ref="B3:B61" si="0">600*1.16^A3</f>
         <v>807.3599999999999</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:D50" si="1">B3/60</f>
         <v>13.455999999999998</v>
       </c>
@@ -463,17 +486,21 @@
         <f t="shared" si="1"/>
         <v>0.22426666666666664</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E66" si="2">D3/24</f>
+        <v>9.3444444444444434E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A61" si="2">A3+1</f>
+        <f t="shared" ref="A4:A67" si="3">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f t="shared" si="0"/>
         <v>936.53759999999988</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <f t="shared" si="1"/>
         <v>15.608959999999998</v>
       </c>
@@ -481,17 +508,21 @@
         <f t="shared" si="1"/>
         <v>0.26014933333333329</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0839555555555554E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f t="shared" si="0"/>
         <v>1086.3836159999998</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f t="shared" si="1"/>
         <v>18.106393599999997</v>
       </c>
@@ -499,17 +530,21 @@
         <f t="shared" si="1"/>
         <v>0.30177322666666662</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2573884444444442E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <f t="shared" si="0"/>
         <v>1260.2049945599997</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f t="shared" si="1"/>
         <v>21.003416575999996</v>
       </c>
@@ -517,17 +552,21 @@
         <f t="shared" si="1"/>
         <v>0.35005694293333328</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4585705955555554E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>1461.8377936895997</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f t="shared" si="1"/>
         <v>24.363963228159996</v>
       </c>
@@ -535,17 +574,21 @@
         <f t="shared" si="1"/>
         <v>0.40606605380266658</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.691941890844444E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>1695.7318406799354</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f t="shared" si="1"/>
         <v>28.262197344665591</v>
       </c>
@@ -553,17 +596,21 @@
         <f t="shared" si="1"/>
         <v>0.47103662241109318</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.962652593379555E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>1967.0489351887252</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f t="shared" si="1"/>
         <v>32.78414891981209</v>
       </c>
@@ -571,17 +618,21 @@
         <f t="shared" si="1"/>
         <v>0.54640248199686814</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2766770083202839E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>2281.776764818921</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f t="shared" si="1"/>
         <v>38.029612746982018</v>
       </c>
@@ -589,17 +640,21 @@
         <f t="shared" si="1"/>
         <v>0.63382687911636693</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6409453296515287E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>2646.8610471899483</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f t="shared" si="1"/>
         <v>44.114350786499138</v>
       </c>
@@ -607,17 +662,21 @@
         <f t="shared" si="1"/>
         <v>0.73523917977498565</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0634965823957735E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>3070.3588147403398</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <f t="shared" si="1"/>
         <v>51.172646912338998</v>
       </c>
@@ -625,17 +684,21 @@
         <f t="shared" si="1"/>
         <v>0.85287744853898328</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5536560355790968E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>3561.6162250987941</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f t="shared" si="1"/>
         <v>59.360270418313235</v>
       </c>
@@ -643,17 +706,21 @@
         <f t="shared" si="1"/>
         <v>0.98933784030522054</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1222410012717522E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>4131.4748211146007</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f t="shared" si="1"/>
         <v>68.857913685243346</v>
       </c>
@@ -661,17 +728,21 @@
         <f t="shared" si="1"/>
         <v>1.1476318947540558</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>4.7817995614752327E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>4792.5107924929371</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
         <v>79.875179874882278</v>
       </c>
@@ -679,17 +750,21 @@
         <f t="shared" si="1"/>
         <v>1.3312529979147045</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5468874913112691E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>5559.3125192918069</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <f t="shared" si="1"/>
         <v>92.655208654863443</v>
       </c>
@@ -697,17 +772,21 @@
         <f t="shared" si="1"/>
         <v>1.5442534775810575</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4343894899210732E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+1</f>
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>6448.8025223784953</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <f t="shared" si="1"/>
         <v>107.48004203964159</v>
       </c>
@@ -715,17 +794,21 @@
         <f t="shared" si="1"/>
         <v>1.7913340339940265</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>7.4638918083084441E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>7480.6109259590548</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f t="shared" si="1"/>
         <v>124.67684876598425</v>
       </c>
@@ -733,17 +816,21 @@
         <f t="shared" si="1"/>
         <v>2.0779474794330706</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>8.6581144976377936E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>8677.5086741125033</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <f t="shared" si="1"/>
         <v>144.62514456854171</v>
       </c>
@@ -751,17 +838,21 @@
         <f t="shared" si="1"/>
         <v>2.4104190761423618</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10043412817259841</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <f t="shared" si="0"/>
         <v>10065.910061970502</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <f t="shared" si="1"/>
         <v>167.76516769950837</v>
       </c>
@@ -769,17 +860,21 @@
         <f t="shared" si="1"/>
         <v>2.7960861283251393</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11650358868021414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <f t="shared" si="0"/>
         <v>11676.455671885782</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <f t="shared" si="1"/>
         <v>194.6075945314297</v>
       </c>
@@ -787,17 +882,21 @@
         <f t="shared" si="1"/>
         <v>3.2434599088571616</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1351441628690484</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <f t="shared" si="0"/>
         <v>13544.688579387508</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <f t="shared" si="1"/>
         <v>225.74480965645847</v>
       </c>
@@ -805,17 +904,21 @@
         <f t="shared" si="1"/>
         <v>3.7624134942743077</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <f t="shared" si="2"/>
+        <v>0.15676722892809616</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <f t="shared" si="0"/>
         <v>15711.83875208951</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <f t="shared" si="1"/>
         <v>261.86397920149182</v>
       </c>
@@ -823,17 +926,21 @@
         <f t="shared" si="1"/>
         <v>4.3643996533581966</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <f t="shared" si="2"/>
+        <v>0.18184998555659151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <f t="shared" si="0"/>
         <v>18225.73295242383</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <f t="shared" si="1"/>
         <v>303.7622158737305</v>
       </c>
@@ -841,17 +948,21 @@
         <f t="shared" si="1"/>
         <v>5.0627035978955082</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21094598324564617</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <f t="shared" si="0"/>
         <v>21141.850224811642</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <f t="shared" si="1"/>
         <v>352.36417041352735</v>
       </c>
@@ -859,17 +970,21 @@
         <f t="shared" si="1"/>
         <v>5.8727361735587893</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.24469734056494954</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <f t="shared" si="0"/>
         <v>24524.546260781502</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <f t="shared" si="1"/>
         <v>408.7424376796917</v>
       </c>
@@ -877,17 +992,21 @@
         <f t="shared" si="1"/>
         <v>6.8123739613281948</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.28384891505534143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <f t="shared" si="0"/>
         <v>28448.473662506542</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <f t="shared" si="1"/>
         <v>474.14122770844239</v>
       </c>
@@ -895,17 +1014,21 @@
         <f t="shared" si="1"/>
         <v>7.9023537951407068</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.3292647414641961</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <f t="shared" si="0"/>
         <v>33000.229448507591</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <f t="shared" si="1"/>
         <v>550.00382414179319</v>
       </c>
@@ -913,17 +1036,21 @@
         <f t="shared" si="1"/>
         <v>9.1667304023632195</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1">
+        <f t="shared" si="2"/>
+        <v>0.3819471000984675</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <f t="shared" si="0"/>
         <v>38280.266160268802</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <f t="shared" si="1"/>
         <v>638.00443600448</v>
       </c>
@@ -931,17 +1058,21 @@
         <f t="shared" si="1"/>
         <v>10.633407266741333</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <f t="shared" si="2"/>
+        <v>0.44305863611422219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <f t="shared" si="0"/>
         <v>44405.108745911806</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <f t="shared" si="1"/>
         <v>740.08514576519678</v>
       </c>
@@ -949,17 +1080,21 @@
         <f t="shared" si="1"/>
         <v>12.334752429419947</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <f t="shared" si="2"/>
+        <v>0.51394801789249778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>51509.926145257697</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <f t="shared" si="1"/>
         <v>858.49876908762826</v>
       </c>
@@ -967,17 +1102,21 @@
         <f t="shared" si="1"/>
         <v>14.308312818127138</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <f t="shared" si="2"/>
+        <v>0.59617970075529747</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <f t="shared" si="0"/>
         <v>59751.514328498917</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <f t="shared" si="1"/>
         <v>995.85857214164866</v>
       </c>
@@ -985,17 +1124,21 @@
         <f t="shared" si="1"/>
         <v>16.597642869027478</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <f t="shared" si="2"/>
+        <v>0.69156845287614488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <f t="shared" si="0"/>
         <v>69311.756621058739</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <f t="shared" si="1"/>
         <v>1155.1959436843124</v>
       </c>
@@ -1003,17 +1146,21 @@
         <f t="shared" si="1"/>
         <v>19.253265728071874</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
+        <f t="shared" si="2"/>
+        <v>0.80221940533632807</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <f t="shared" si="0"/>
         <v>80401.637680428132</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <f t="shared" si="1"/>
         <v>1340.0272946738021</v>
       </c>
@@ -1021,17 +1168,21 @@
         <f t="shared" si="1"/>
         <v>22.333788244563369</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <f t="shared" si="2"/>
+        <v>0.93057451019014037</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <f t="shared" si="0"/>
         <v>93265.899709296646</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <f t="shared" si="1"/>
         <v>1554.4316618216108</v>
       </c>
@@ -1039,17 +1190,21 @@
         <f t="shared" si="1"/>
         <v>25.907194363693513</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0794664318205631</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <f t="shared" si="0"/>
         <v>108188.44366278409</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <f t="shared" si="1"/>
         <v>1803.1407277130681</v>
       </c>
@@ -1057,17 +1212,21 @@
         <f t="shared" si="1"/>
         <v>30.052345461884467</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2521810609118529</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <f t="shared" si="0"/>
         <v>125498.59464882954</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <f t="shared" si="1"/>
         <v>2091.6432441471593</v>
       </c>
@@ -1075,17 +1234,21 @@
         <f t="shared" si="1"/>
         <v>34.860720735785989</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4525300306577495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <f t="shared" si="0"/>
         <v>145578.36979264228</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <f t="shared" si="1"/>
         <v>2426.3061632107047</v>
       </c>
@@ -1093,17 +1256,21 @@
         <f t="shared" si="1"/>
         <v>40.438436053511744</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6849348355629894</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <f t="shared" si="0"/>
         <v>168870.90895946504</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <f t="shared" si="1"/>
         <v>2814.5151493244175</v>
       </c>
@@ -1111,17 +1278,21 @@
         <f t="shared" si="1"/>
         <v>46.908585822073626</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9545244092530678</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <f t="shared" si="0"/>
         <v>195890.25439297943</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <f t="shared" si="1"/>
         <v>3264.837573216324</v>
       </c>
@@ -1129,17 +1300,21 @@
         <f t="shared" si="1"/>
         <v>54.413959553605402</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2672483147335583</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <f t="shared" si="0"/>
         <v>227232.69509585612</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <f t="shared" si="1"/>
         <v>3787.2115849309353</v>
       </c>
@@ -1147,17 +1322,21 @@
         <f t="shared" si="1"/>
         <v>63.120193082182254</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6300080450909271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <f t="shared" si="0"/>
         <v>263589.92631119309</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <f t="shared" si="1"/>
         <v>4393.1654385198844</v>
       </c>
@@ -1165,17 +1344,21 @@
         <f t="shared" si="1"/>
         <v>73.219423975331409</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0508093323054752</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <f t="shared" si="0"/>
         <v>305764.31452098401</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <f t="shared" si="1"/>
         <v>5096.0719086830668</v>
       </c>
@@ -1183,17 +1366,21 @@
         <f t="shared" si="1"/>
         <v>84.934531811384446</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5389388254743519</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <f t="shared" si="0"/>
         <v>354686.6048443414</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <f t="shared" si="1"/>
         <v>5911.443414072357</v>
       </c>
@@ -1201,17 +1388,21 @@
         <f t="shared" si="1"/>
         <v>98.524056901205952</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1051690375502483</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <f t="shared" si="0"/>
         <v>411436.46161943604</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <f t="shared" si="1"/>
         <v>6857.2743603239342</v>
       </c>
@@ -1219,17 +1410,21 @@
         <f t="shared" si="1"/>
         <v>114.28790600539891</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <f t="shared" si="2"/>
+        <v>4.7619960835582882</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <f t="shared" si="0"/>
         <v>477266.29547854571</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <f t="shared" si="1"/>
         <v>7954.4382579757621</v>
       </c>
@@ -1237,17 +1432,21 @@
         <f t="shared" si="1"/>
         <v>132.57397096626269</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5239154569276119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <f t="shared" si="0"/>
         <v>553628.90275511297</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <f t="shared" si="1"/>
         <v>9227.1483792518829</v>
       </c>
@@ -1255,17 +1454,21 @@
         <f t="shared" si="1"/>
         <v>153.78580632086471</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4077419300360292</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <f t="shared" si="0"/>
         <v>642209.52719593106</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <f t="shared" si="1"/>
         <v>10703.492119932185</v>
       </c>
@@ -1273,17 +1476,21 @@
         <f t="shared" si="1"/>
         <v>178.39153533220309</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <f t="shared" si="2"/>
+        <v>7.4329806388417952</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <f t="shared" si="0"/>
         <v>744963.05154728016</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <f t="shared" si="1"/>
         <v>12416.050859121337</v>
       </c>
@@ -1291,17 +1498,21 @@
         <f t="shared" si="1"/>
         <v>206.9341809853556</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <f t="shared" si="2"/>
+        <v>8.6222575410564826</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <f t="shared" si="0"/>
         <v>864157.1397948449</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <f t="shared" si="1"/>
         <v>14402.618996580748</v>
       </c>
@@ -1309,203 +1520,808 @@
         <f t="shared" si="1"/>
         <v>240.04364994301247</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <f t="shared" si="2"/>
+        <v>10.001818747625519</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <f t="shared" si="0"/>
         <v>1002422.28216202</v>
       </c>
-      <c r="C51" s="2">
-        <f t="shared" ref="C51:D51" si="3">B51/60</f>
+      <c r="C51" s="1">
+        <f t="shared" ref="C51:D51" si="4">B51/60</f>
         <v>16707.038036033668</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>278.45063393389444</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <f t="shared" si="2"/>
+        <v>11.602109747245601</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <f t="shared" si="0"/>
         <v>1162809.847307943</v>
       </c>
-      <c r="C52" s="2">
-        <f t="shared" ref="C52:D52" si="4">B52/60</f>
+      <c r="C52" s="1">
+        <f t="shared" ref="C52:D52" si="5">B52/60</f>
         <v>19380.164121799051</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>323.00273536331753</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <f t="shared" si="2"/>
+        <v>13.458447306804898</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <f t="shared" si="0"/>
         <v>1348859.4228772139</v>
       </c>
-      <c r="C53" s="2">
-        <f t="shared" ref="C53:D53" si="5">B53/60</f>
+      <c r="C53" s="1">
+        <f t="shared" ref="C53:D53" si="6">B53/60</f>
         <v>22480.990381286898</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>374.68317302144828</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <f t="shared" si="2"/>
+        <v>15.611798875893678</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <f t="shared" si="0"/>
         <v>1564676.9305375682</v>
       </c>
-      <c r="C54" s="2">
-        <f t="shared" ref="C54:D54" si="6">B54/60</f>
+      <c r="C54" s="1">
+        <f t="shared" ref="C54:D54" si="7">B54/60</f>
         <v>26077.948842292804</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>434.63248070488009</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <f t="shared" si="2"/>
+        <v>18.109686696036672</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <f t="shared" si="0"/>
         <v>1815025.2394235793</v>
       </c>
-      <c r="C55" s="2">
-        <f t="shared" ref="C55:D55" si="7">B55/60</f>
+      <c r="C55" s="1">
+        <f t="shared" ref="C55:D55" si="8">B55/60</f>
         <v>30250.420657059654</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>504.17367761766093</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <f t="shared" si="2"/>
+        <v>21.00723656740254</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <f t="shared" si="0"/>
         <v>2105429.2777313516</v>
       </c>
-      <c r="C56" s="2">
-        <f t="shared" ref="C56:D56" si="8">B56/60</f>
+      <c r="C56" s="1">
+        <f t="shared" ref="C56:D56" si="9">B56/60</f>
         <v>35090.487962189196</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>584.84146603648662</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <f t="shared" si="2"/>
+        <v>24.368394418186941</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <f t="shared" si="0"/>
         <v>2442297.9621683676</v>
       </c>
-      <c r="C57" s="2">
-        <f t="shared" ref="C57:D57" si="9">B57/60</f>
+      <c r="C57" s="1">
+        <f t="shared" ref="C57:D57" si="10">B57/60</f>
         <v>40704.966036139456</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>678.41610060232426</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <f t="shared" si="2"/>
+        <v>28.267337525096845</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <f t="shared" si="0"/>
         <v>2833065.6361153065</v>
       </c>
-      <c r="C58" s="2">
-        <f t="shared" ref="C58:D58" si="10">B58/60</f>
+      <c r="C58" s="1">
+        <f t="shared" ref="C58:D58" si="11">B58/60</f>
         <v>47217.760601921778</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>786.96267669869633</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <f t="shared" si="2"/>
+        <v>32.790111529112345</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <f t="shared" si="0"/>
         <v>3286356.1378937555</v>
       </c>
-      <c r="C59" s="2">
-        <f t="shared" ref="C59:D59" si="11">B59/60</f>
+      <c r="C59" s="1">
+        <f t="shared" ref="C59:D59" si="12">B59/60</f>
         <v>54772.602298229256</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>912.87670497048759</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <f t="shared" si="2"/>
+        <v>38.036529373770314</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <f t="shared" si="0"/>
         <v>3812173.119956756</v>
       </c>
-      <c r="C60" s="2">
-        <f t="shared" ref="C60:D60" si="12">B60/60</f>
+      <c r="C60" s="1">
+        <f t="shared" ref="C60:D60" si="13">B60/60</f>
         <v>63536.218665945933</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1058.9369777657655</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <f t="shared" si="2"/>
+        <v>44.12237407357356</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <f t="shared" si="0"/>
         <v>4422120.8191498369</v>
       </c>
-      <c r="C61" s="2">
-        <f t="shared" ref="C61:D61" si="13">B61/60</f>
+      <c r="C61" s="1">
+        <f t="shared" ref="C61:D62" si="14">B61/60</f>
         <v>73702.013652497277</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1228.3668942082879</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="2"/>
+        <v>51.181953925345333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="5">
+        <f>600*1.16^A62 + ((24*60*60*60)*(A62-60))</f>
+        <v>10313660.150213812</v>
+      </c>
+      <c r="C62" s="5">
+        <f t="shared" si="14"/>
+        <v>171894.33583689685</v>
+      </c>
+      <c r="D62" s="5">
+        <f t="shared" si="14"/>
+        <v>2864.9055972816141</v>
+      </c>
+      <c r="E62" s="5">
+        <f t="shared" si="2"/>
+        <v>119.37106655340058</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" ref="B63:B81" si="15">600*1.16^A63 + ((24*60*60*60)*(A63-60))</f>
+        <v>16318405.774248019</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" ref="C63:D63" si="16">B63/60</f>
+        <v>271973.42957080033</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="16"/>
+        <v>4532.8904928466718</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="2"/>
+        <v>188.87043720194467</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" si="15"/>
+        <v>22454470.698127702</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" ref="C64:D64" si="17">B64/60</f>
+        <v>374241.17830212839</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="17"/>
+        <v>6237.3529717021402</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="2"/>
+        <v>259.88970715425586</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <f t="shared" si="15"/>
+        <v>28742866.009828135</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" ref="C65:D65" si="18">B65/60</f>
+        <v>479047.7668304689</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="18"/>
+        <v>7984.1294471744814</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="2"/>
+        <v>332.67206029893674</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <f t="shared" si="15"/>
+        <v>35207964.571400635</v>
+      </c>
+      <c r="C66" s="1">
+        <f t="shared" ref="C66:D66" si="19">B66/60</f>
+        <v>586799.4095233439</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="19"/>
+        <v>9779.9901587223976</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" si="2"/>
+        <v>407.49958994676655</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <f t="shared" si="15"/>
+        <v>41878038.902824737</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" ref="C67:D67" si="20">B67/60</f>
+        <v>697967.315047079</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" si="20"/>
+        <v>11632.788584117983</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" ref="E67:E81" si="21">D67/24</f>
+        <v>484.69952433824932</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" ref="A68:A100" si="22">A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <f t="shared" si="15"/>
+        <v>48785885.127276696</v>
+      </c>
+      <c r="C68" s="1">
+        <f t="shared" ref="C68:D68" si="23">B68/60</f>
+        <v>813098.08545461157</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="23"/>
+        <v>13551.63475757686</v>
+      </c>
+      <c r="E68" s="1">
+        <f t="shared" si="21"/>
+        <v>564.65144823236915</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="22"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <f t="shared" si="15"/>
+        <v>55969546.747640967</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" ref="C69:D69" si="24">B69/60</f>
+        <v>932825.77912734949</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="24"/>
+        <v>15547.096318789158</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="21"/>
+        <v>647.79567994954823</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="22"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <f t="shared" si="15"/>
+        <v>63473154.227263525</v>
+      </c>
+      <c r="C70" s="1">
+        <f t="shared" ref="C70:D70" si="25">B70/60</f>
+        <v>1057885.9037877254</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="25"/>
+        <v>17631.431729795422</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" si="21"/>
+        <v>734.64298874147596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="22"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
+        <f t="shared" si="15"/>
+        <v>71347898.903625682</v>
+      </c>
+      <c r="C71" s="1">
+        <f t="shared" ref="C71:D71" si="26">B71/60</f>
+        <v>1189131.6483937614</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="26"/>
+        <v>19818.86080656269</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="21"/>
+        <v>825.7858669401121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="22"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <f t="shared" si="15"/>
+        <v>79653162.728205785</v>
+      </c>
+      <c r="C72" s="1">
+        <f t="shared" ref="C72:D72" si="27">B72/60</f>
+        <v>1327552.7121367631</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="27"/>
+        <v>22125.878535612719</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" si="21"/>
+        <v>921.91160565052996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="22"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <f t="shared" si="15"/>
+        <v>88457828.764718711</v>
+      </c>
+      <c r="C73" s="1">
+        <f t="shared" ref="C73:D73" si="28">B73/60</f>
+        <v>1474297.1460786453</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="28"/>
+        <v>24571.619101310753</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="21"/>
+        <v>1023.8174625546147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="22"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <f t="shared" si="15"/>
+        <v>97841801.367073715</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" ref="C74:D74" si="29">B74/60</f>
+        <v>1630696.6894512286</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="29"/>
+        <v>27178.278157520475</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="21"/>
+        <v>1132.4282565633532</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="22"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="1">
+        <f t="shared" si="15"/>
+        <v>107897769.58580551</v>
+      </c>
+      <c r="C75" s="1">
+        <f t="shared" ref="C75:D75" si="30">B75/60</f>
+        <v>1798296.1597634251</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="30"/>
+        <v>29971.602662723752</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="21"/>
+        <v>1248.8167776134896</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="22"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="1">
+        <f t="shared" si="15"/>
+        <v>118733252.71953438</v>
+      </c>
+      <c r="C76" s="1">
+        <f t="shared" ref="C76:D76" si="31">B76/60</f>
+        <v>1978887.5453255731</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="31"/>
+        <v>32981.459088759548</v>
+      </c>
+      <c r="E76" s="1">
+        <f t="shared" si="21"/>
+        <v>1374.2274620316477</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="22"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="1">
+        <f t="shared" si="15"/>
+        <v>130472973.15465987</v>
+      </c>
+      <c r="C77" s="1">
+        <f t="shared" ref="C77:D77" si="32">B77/60</f>
+        <v>2174549.5525776646</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="32"/>
+        <v>36242.492542961074</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="21"/>
+        <v>1510.1038559567114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="22"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="1">
+        <f t="shared" si="15"/>
+        <v>143261608.85940546</v>
+      </c>
+      <c r="C78" s="1">
+        <f t="shared" ref="C78:D78" si="33">B78/60</f>
+        <v>2387693.4809900909</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="33"/>
+        <v>39794.891349834848</v>
+      </c>
+      <c r="E78" s="1">
+        <f t="shared" si="21"/>
+        <v>1658.1204729097853</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="22"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="1">
+        <f t="shared" si="15"/>
+        <v>157266986.27691033</v>
+      </c>
+      <c r="C79" s="1">
+        <f t="shared" ref="C79:D79" si="34">B79/60</f>
+        <v>2621116.4379485054</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="34"/>
+        <v>43685.273965808425</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="21"/>
+        <v>1820.2197485753511</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="22"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="1">
+        <f t="shared" si="15"/>
+        <v>172683784.08121598</v>
+      </c>
+      <c r="C80" s="1">
+        <f t="shared" ref="C80:D80" si="35">B80/60</f>
+        <v>2878063.0680202665</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="35"/>
+        <v>47967.717800337778</v>
+      </c>
+      <c r="E80" s="1">
+        <f t="shared" si="21"/>
+        <v>1998.6549083474074</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="22"/>
+        <v>80</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" si="15"/>
+        <v>189737829.5342105</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ref="C81:D81" si="36">B81/60</f>
+        <v>3162297.1589035084</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="36"/>
+        <v>52704.952648391809</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="21"/>
+        <v>2196.039693682992</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="22"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="22"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="22"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="22"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f t="shared" si="22"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="22"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="22"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="22"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="22"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="22"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="22"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="22"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="22"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="22"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="22"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="22"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f t="shared" si="22"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f t="shared" si="22"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f t="shared" si="22"/>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>